<commit_message>
Boundary value analysis new version
</commit_message>
<xml_diff>
--- a/Testexercise5.xlsx
+++ b/Testexercise5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compi_000\PycharmProjects\Easterdiscount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8B97C8-9A6C-45FC-8C78-CD6A54C06126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65864573-7685-4985-A0CC-7880EC14B763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F980F882-87B9-47A3-AE88-3FDCC301FD98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -76,12 +76,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>representative</t>
-  </si>
-  <si>
-    <t>]0,…50]</t>
-  </si>
-  <si>
     <t>[50.01…..100]</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>[9/04/2022 ….....18/04/2022]</t>
   </si>
   <si>
-    <t>[min_Decimal…...0]</t>
-  </si>
-  <si>
     <t>vEP2_2</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>During easter holiday, second tier</t>
   </si>
   <si>
-    <t>Between 9-18 April 2022 and total is from 100,01, discount 15%</t>
-  </si>
-  <si>
     <t>Between 9-18 April 2022, Total is  between 50,01-100, discount 10%</t>
   </si>
   <si>
@@ -166,9 +154,6 @@
     <t>During easter holiday, third tier</t>
   </si>
   <si>
-    <t>During easter holiday, first tier</t>
-  </si>
-  <si>
     <t>Earlier than easter holiday, first tier</t>
   </si>
   <si>
@@ -232,17 +217,80 @@
     <t>ValueError:The day given is not of type date</t>
   </si>
   <si>
+    <t>Total is with a precision greater than two- no discount</t>
+  </si>
+  <si>
+    <t>If the function is called with a total with a precision greater than 2,  it will be truncated before price calculation. After that the function calculates the price with 15% discount.</t>
+  </si>
+  <si>
+    <t>If the function is called with a total with a precision greater than 2,  it will be truncated before price calculation. Date out of the eastern perid, the function do not reduce the price.</t>
+  </si>
+  <si>
+    <t>[0,…50]</t>
+  </si>
+  <si>
+    <t>[min_Decimal…...0[</t>
+  </si>
+  <si>
+    <t>representative1-BVA</t>
+  </si>
+  <si>
+    <t>representative2-BVA</t>
+  </si>
+  <si>
+    <t>representative3-EP</t>
+  </si>
+  <si>
+    <t>50.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>88.99.7777</t>
+  </si>
+  <si>
+    <t>00.00.0000</t>
+  </si>
+  <si>
+    <t>Boundari value test, Total=0</t>
+  </si>
+  <si>
+    <t>Exercise5/vEP1_1</t>
+  </si>
+  <si>
+    <t>During easter holiday, first tier, Boundari value test</t>
+  </si>
+  <si>
+    <t>Equivalence test, first tier, in eastern period</t>
+  </si>
+  <si>
+    <t>In easter holiday, second tier</t>
+  </si>
+  <si>
+    <t>In easter holiday and total between 50,01-100 Eur, 10% discount</t>
+  </si>
+  <si>
+    <t>Exercise5/vEP1_2</t>
+  </si>
+  <si>
+    <t>In easter holiday, third tier</t>
+  </si>
+  <si>
+    <t>Between 9-18 April 2022 and total is bigger than 100, discount 15%</t>
+  </si>
+  <si>
     <t>Total is with a precision 
-greater than two-third tier</t>
-  </si>
-  <si>
-    <t>Total is with a precision greater than two- no discount</t>
-  </si>
-  <si>
-    <t>If the function is called with a total with a precision greater than 2,  it will be truncated before price calculation. After that the function calculates the price with 15% discount.</t>
-  </si>
-  <si>
-    <t>If the function is called with a total with a precision greater than 2,  it will be truncated before price calculation. Date out of the eastern perid, the function do not reduce the price.</t>
+greater than two, third tier</t>
+  </si>
+  <si>
+    <t>Total in not allowed format, float</t>
+  </si>
+  <si>
+    <t>The function has to be called with total in type of decimal.</t>
+  </si>
+  <si>
+    <t>Exercise5/iEP1_2</t>
   </si>
 </sst>
 </file>
@@ -690,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76080AAE-91CC-4536-8750-B6AE5B58BDF7}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -741,13 +789,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -770,13 +818,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>5</v>
@@ -799,10 +847,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
@@ -828,10 +876,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>6</v>
@@ -857,10 +905,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
@@ -886,10 +934,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>6</v>
@@ -915,10 +963,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
@@ -944,10 +992,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>6</v>
@@ -973,10 +1021,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>6</v>
@@ -1002,10 +1050,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>6</v>
@@ -1014,13 +1062,13 @@
         <v>5</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G11" s="20">
         <v>44660</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1031,10 +1079,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>6</v>
@@ -1049,7 +1097,7 @@
         <v>44661</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1060,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>6</v>
@@ -1075,10 +1123,10 @@
         <v>100</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -1089,10 +1137,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>6</v>
@@ -1118,10 +1166,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>6</v>
@@ -1141,6 +1189,180 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>44662</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7">
+        <v>20</v>
+      </c>
+      <c r="G17" s="20">
+        <v>44663</v>
+      </c>
+      <c r="H17" s="7">
+        <v>19</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4">
+        <v>50.01</v>
+      </c>
+      <c r="G18" s="12">
+        <v>44668</v>
+      </c>
+      <c r="H18" s="4">
+        <v>45</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="7">
+        <v>70</v>
+      </c>
+      <c r="G19" s="20">
+        <v>44667</v>
+      </c>
+      <c r="H19" s="7">
+        <v>63</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4">
+        <v>120</v>
+      </c>
+      <c r="G20" s="12">
+        <v>44669</v>
+      </c>
+      <c r="H20" s="4">
+        <v>102</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7">
+        <v>120.09999000000001</v>
+      </c>
+      <c r="G21" s="20">
+        <v>44660</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1150,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E64B6B9-ADBF-4B1D-B7B6-80EE0B4335B7}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1162,7 +1384,7 @@
     <col min="3" max="3" width="27.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
@@ -1171,131 +1393,181 @@
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0</v>
+      </c>
+      <c r="E2" s="14">
+        <v>50</v>
+      </c>
+      <c r="F2" s="14">
         <v>20</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="21"/>
       <c r="B3" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="14">
+        <v>13</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="14">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F3" s="14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>
       <c r="B4" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="21"/>
       <c r="B5" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="21"/>
       <c r="B6" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="21"/>
       <c r="B7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="15">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
-        <v>27</v>
-      </c>
       <c r="B8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="16">
         <v>44660</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="16">
+        <v>44669</v>
+      </c>
+      <c r="F8" s="16">
+        <v>44667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
       <c r="B9" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="16">
+        <v>34</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16">
         <v>44659</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F9" s="16">
+        <v>44628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
       <c r="B10" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="16">
         <v>44670</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" s="16"/>
+      <c r="F10" s="16">
+        <v>44676</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="21"/>
       <c r="B11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1304,6 +1576,6 @@
     <mergeCell ref="A8:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final version including 20 Test cases
</commit_message>
<xml_diff>
--- a/Testexercise5.xlsx
+++ b/Testexercise5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compi_000\PycharmProjects\Easterdiscount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65864573-7685-4985-A0CC-7880EC14B763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFE4C84-2FC0-4561-B2BF-8A1643B0E1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F980F882-87B9-47A3-AE88-3FDCC301FD98}"/>
   </bookViews>
@@ -253,13 +253,7 @@
     <t>00.00.0000</t>
   </si>
   <si>
-    <t>Boundari value test, Total=0</t>
-  </si>
-  <si>
     <t>Exercise5/vEP1_1</t>
-  </si>
-  <si>
-    <t>During easter holiday, first tier, Boundari value test</t>
   </si>
   <si>
     <t>Equivalence test, first tier, in eastern period</t>
@@ -287,10 +281,16 @@
     <t>Total in not allowed format, float</t>
   </si>
   <si>
-    <t>The function has to be called with total in type of decimal.</t>
-  </si>
-  <si>
     <t>Exercise5/iEP1_2</t>
+  </si>
+  <si>
+    <t>Boundary value test, Total=0</t>
+  </si>
+  <si>
+    <t>During easter holiday, first tier, Boundary value test</t>
+  </si>
+  <si>
+    <t>The argument total has a type of float.</t>
   </si>
 </sst>
 </file>
@@ -741,7 +741,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,13 +789,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -824,7 +824,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>5</v>
@@ -850,7 +850,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
@@ -1137,7 +1137,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>61</v>
@@ -1195,13 +1195,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>5</v>
@@ -1224,13 +1224,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>5</v>
@@ -1253,13 +1253,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>5</v>
@@ -1282,13 +1282,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>5</v>
@@ -1311,10 +1311,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>6</v>
@@ -1340,13 +1340,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
program calculate_price_test is optimized and additional one test case is added for testing what happened if total is a float.
</commit_message>
<xml_diff>
--- a/Testexercise5.xlsx
+++ b/Testexercise5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compi_000\PycharmProjects\Easterdiscount\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFE4C84-2FC0-4561-B2BF-8A1643B0E1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC4F9FC-5E15-4E58-888A-8C00BB75FE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F980F882-87B9-47A3-AE88-3FDCC301FD98}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>The argument total has a type of float.</t>
+  </si>
+  <si>
+    <t>0 on first day</t>
+  </si>
+  <si>
+    <t>Between 9-18 April,  total=0</t>
   </si>
 </sst>
 </file>
@@ -738,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76080AAE-91CC-4536-8750-B6AE5B58BDF7}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,7 +926,7 @@
         <v>50.01</v>
       </c>
       <c r="G6" s="12">
-        <v>44562</v>
+        <v>44296</v>
       </c>
       <c r="H6" s="4">
         <v>50.01</v>
@@ -1363,6 +1369,35 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>44660</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>